<commit_message>
Updated pushbutton part #
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29060" windowHeight="18300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>McMaster</t>
   </si>
@@ -66,12 +66,6 @@
     <t>http://www.digikey.com/product-search/en?keywords=ATTINY85-20PU-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?keywords=CKN9074-ND</t>
-  </si>
-  <si>
-    <t>Might need taller height</t>
-  </si>
-  <si>
     <t>2.2k SMD resistors</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
   </si>
   <si>
     <t>Center positive</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-search/en?keywords=450-1642-ND</t>
   </si>
 </sst>
 </file>
@@ -689,7 +686,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -728,7 +725,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -745,15 +742,15 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -770,15 +767,15 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -795,10 +792,10 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -866,31 +863,28 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" s="3">
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>0.72</v>
+        <v>0.4</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
-        <v>16</v>
-      </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -907,15 +901,15 @@
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -931,12 +925,12 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -952,23 +946,23 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -981,12 +975,12 @@
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1003,19 +997,19 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="C16" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="2">
         <f>SUM(D2:D14)</f>
-        <v>19.244200000000003</v>
+        <v>18.924200000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>